<commit_message>
made the music module
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Class Hw\CS145\ARV-TONES\ARV-TONES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Atmel Studio\7.0\GccApplication3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08F405BB-7756-4C84-9C28-A2481A7AF415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02872C56-6D76-4953-9AE3-8FA4638DBA53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-480000" yWindow="-480000" windowWidth="2400" windowHeight="585" xr2:uid="{CF926C44-2E5F-4C19-9C24-B048CD17F12D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{CF926C44-2E5F-4C19-9C24-B048CD17F12D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -78,6 +76,9 @@
   </si>
   <si>
     <t>Frequency</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -436,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60C913B-E659-40D1-A92A-A3DD20215290}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +450,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F1" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -480,35 +481,35 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="C3">
-        <f>440*2^(B3/12)</f>
-        <v>440</v>
+        <f t="shared" ref="C3:C14" si="0">440*2^(B3/12)</f>
+        <v>220</v>
       </c>
       <c r="D3">
-        <f>1/C3</f>
+        <f t="shared" ref="D3:D14" si="1">1/C3</f>
+        <v>4.5454545454545452E-3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E14" si="2">D3/2</f>
         <v>2.2727272727272726E-3</v>
       </c>
-      <c r="E3">
-        <f>D3/2</f>
-        <v>1.1363636363636363E-3</v>
-      </c>
       <c r="F3">
-        <f>ROUND(E3/$F$1,0)</f>
-        <v>114</v>
+        <f t="shared" ref="F3:F14" si="3">ROUND(E3/$F$1,0)</f>
+        <v>2273</v>
       </c>
       <c r="G3">
-        <f>F3*$F$1</f>
-        <v>1.1400000000000002E-3</v>
+        <f t="shared" ref="G3:G14" si="4">F3*$F$1</f>
+        <v>2.2729999999999998E-3</v>
       </c>
       <c r="H3">
-        <f>G3*2</f>
-        <v>2.2800000000000003E-3</v>
+        <f t="shared" ref="H3:H14" si="5">G3*2</f>
+        <v>4.5459999999999997E-3</v>
       </c>
       <c r="I3">
-        <f>1/H3</f>
-        <v>438.59649122807014</v>
+        <f t="shared" ref="I3:I14" si="6">1/H3</f>
+        <v>219.9736031676199</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -516,35 +517,35 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>-11</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C13" si="0">440*2^(B4/12)</f>
-        <v>466.16376151808993</v>
+        <f t="shared" si="0"/>
+        <v>233.08188075904496</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D13" si="1">1/C4</f>
+        <f t="shared" si="1"/>
+        <v>4.2903377849167887E-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
         <v>2.1451688924583943E-3</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E13" si="2">D4/2</f>
-        <v>1.0725844462291972E-3</v>
-      </c>
       <c r="F4">
-        <f t="shared" ref="F4:F13" si="3">ROUND(E4/$F$1,0)</f>
-        <v>107</v>
+        <f t="shared" si="3"/>
+        <v>2145</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G13" si="4">F4*$F$1</f>
-        <v>1.07E-3</v>
+        <f t="shared" si="4"/>
+        <v>2.1449999999999998E-3</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H13" si="5">G4*2</f>
-        <v>2.14E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.2899999999999995E-3</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I13" si="6">1/H4</f>
-        <v>467.28971962616822</v>
+        <f t="shared" si="6"/>
+        <v>233.10023310023311</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -552,35 +553,35 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>-10</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>493.88330125612413</v>
+        <v>246.94165062806206</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>2.0247698139553164E-3</v>
+        <v>4.0495396279106328E-3</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>1.0123849069776582E-3</v>
+        <v>2.0247698139553164E-3</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>2025</v>
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>1.01E-3</v>
+        <v>2.0249999999999999E-3</v>
       </c>
       <c r="H5">
         <f t="shared" si="5"/>
-        <v>2.0200000000000001E-3</v>
+        <v>4.0499999999999998E-3</v>
       </c>
       <c r="I5">
         <f t="shared" si="6"/>
-        <v>495.04950495049502</v>
+        <v>246.9135802469136</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -588,35 +589,35 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>-9</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>523.25113060119725</v>
+        <v>261.62556530059862</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.911128216485715E-3</v>
+        <v>3.82225643297143E-3</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>9.555641082428575E-4</v>
+        <v>1.911128216485715E-3</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>96</v>
+        <v>1911</v>
       </c>
       <c r="G6">
         <f t="shared" si="4"/>
-        <v>9.6000000000000013E-4</v>
+        <v>1.9109999999999999E-3</v>
       </c>
       <c r="H6">
         <f t="shared" si="5"/>
-        <v>1.9200000000000003E-3</v>
+        <v>3.8219999999999999E-3</v>
       </c>
       <c r="I6">
         <f t="shared" si="6"/>
-        <v>520.83333333333326</v>
+        <v>261.64311878597596</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -624,35 +625,35 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>-8</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>554.36526195374415</v>
+        <v>277.18263097687208</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1.803864831782045E-3</v>
+        <v>3.60772966356409E-3</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>9.019324158910225E-4</v>
+        <v>1.803864831782045E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>1804</v>
       </c>
       <c r="G7">
         <f t="shared" si="4"/>
-        <v>9.0000000000000008E-4</v>
+        <v>1.8039999999999998E-3</v>
       </c>
       <c r="H7">
         <f t="shared" si="5"/>
-        <v>1.8000000000000002E-3</v>
+        <v>3.6079999999999997E-3</v>
       </c>
       <c r="I7">
         <f t="shared" si="6"/>
-        <v>555.55555555555554</v>
+        <v>277.16186252771621</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -660,35 +661,35 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>587.32953583481515</v>
+        <v>293.66476791740757</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>1.7026216782689563E-3</v>
+        <v>3.4052433565379125E-3</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>8.5131083913447814E-4</v>
+        <v>1.7026216782689563E-3</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>1703</v>
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>8.5000000000000006E-4</v>
+        <v>1.7029999999999999E-3</v>
       </c>
       <c r="H8">
         <f t="shared" si="5"/>
-        <v>1.7000000000000001E-3</v>
+        <v>3.4059999999999997E-3</v>
       </c>
       <c r="I8">
         <f t="shared" si="6"/>
-        <v>588.23529411764707</v>
+        <v>293.59953024075162</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,35 +697,35 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>622.25396744416184</v>
+        <v>311.12698372208087</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>1.6070608663330626E-3</v>
+        <v>3.2141217326661256E-3</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>8.0353043316653129E-4</v>
+        <v>1.6070608663330628E-3</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>1607</v>
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>8.0000000000000004E-4</v>
+        <v>1.6069999999999999E-3</v>
       </c>
       <c r="H9">
         <f t="shared" si="5"/>
-        <v>1.6000000000000001E-3</v>
+        <v>3.2139999999999998E-3</v>
       </c>
       <c r="I9">
         <f t="shared" si="6"/>
-        <v>625</v>
+        <v>311.13876789047919</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -732,143 +733,611 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>659.25511382573984</v>
+        <v>329.62755691286992</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>1.5168634706477664E-3</v>
+        <v>3.0337269412955329E-3</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>7.5843173532388322E-4</v>
+        <v>1.5168634706477664E-3</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>1517</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>7.6000000000000004E-4</v>
+        <v>1.5169999999999999E-3</v>
       </c>
       <c r="H10">
         <f t="shared" si="5"/>
-        <v>1.5200000000000001E-3</v>
+        <v>3.0339999999999998E-3</v>
       </c>
       <c r="I10">
         <f t="shared" si="6"/>
-        <v>657.8947368421052</v>
+        <v>329.59789057350037</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>698.45646286600777</v>
+        <v>349.22823143300388</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>1.4317284657896286E-3</v>
+        <v>2.8634569315792572E-3</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>7.158642328948143E-4</v>
+        <v>1.4317284657896286E-3</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>1432</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>7.2000000000000005E-4</v>
+        <v>1.4319999999999999E-3</v>
       </c>
       <c r="H11">
         <f t="shared" si="5"/>
-        <v>1.4400000000000001E-3</v>
+        <v>2.8639999999999998E-3</v>
       </c>
       <c r="I11">
         <f t="shared" si="6"/>
-        <v>694.44444444444446</v>
+        <v>349.1620111731844</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>-3</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>739.9888454232688</v>
+        <v>369.99442271163446</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>1.3513717215940012E-3</v>
+        <v>2.702743443188002E-3</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>6.7568586079700061E-4</v>
+        <v>1.351371721594001E-3</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>68</v>
+        <v>1351</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>6.8000000000000005E-4</v>
+        <v>1.351E-3</v>
       </c>
       <c r="H12">
         <f t="shared" si="5"/>
-        <v>1.3600000000000001E-3</v>
+        <v>2.702E-3</v>
       </c>
       <c r="I12">
         <f t="shared" si="6"/>
-        <v>735.29411764705878</v>
+        <v>370.09622501850481</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>-2</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>783.99087196349853</v>
+        <v>391.99543598174927</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>1.2755250548970149E-3</v>
+        <v>2.5510501097940298E-3</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>6.3776252744850745E-4</v>
+        <v>1.2755250548970149E-3</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>1276</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>6.4000000000000005E-4</v>
+        <v>1.276E-3</v>
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
-        <v>1.2800000000000001E-3</v>
+        <v>2.552E-3</v>
       </c>
       <c r="I13">
         <f t="shared" si="6"/>
-        <v>781.24999999999989</v>
+        <v>391.84952978056424</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>415.30469757994513</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2.4078706689983982E-3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>1.2039353344991991E-3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>1204</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>1.204E-3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>2.408E-3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>415.28239202657807</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>440*2^(B15/12)</f>
+        <v>440</v>
+      </c>
+      <c r="D15">
+        <f>1/C15</f>
+        <v>2.2727272727272726E-3</v>
+      </c>
+      <c r="E15">
+        <f>D15/2</f>
+        <v>1.1363636363636363E-3</v>
+      </c>
+      <c r="F15">
+        <f>ROUND(E15/$F$1,0)</f>
+        <v>1136</v>
+      </c>
+      <c r="G15">
+        <f>F15*$F$1</f>
+        <v>1.1359999999999999E-3</v>
+      </c>
+      <c r="H15">
+        <f>G15*2</f>
+        <v>2.2719999999999997E-3</v>
+      </c>
+      <c r="I15">
+        <f>1/H15</f>
+        <v>440.14084507042259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C26" si="7">440*2^(B16/12)</f>
+        <v>466.16376151808993</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D26" si="8">1/C16</f>
+        <v>2.1451688924583943E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E26" si="9">D16/2</f>
+        <v>1.0725844462291972E-3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F26" si="10">ROUND(E16/$F$1,0)</f>
+        <v>1073</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G26" si="11">F16*$F$1</f>
+        <v>1.073E-3</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H26" si="12">G16*2</f>
+        <v>2.1459999999999999E-3</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16:I26" si="13">1/H16</f>
+        <v>465.98322460391427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="7"/>
+        <v>493.88330125612413</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="8"/>
+        <v>2.0247698139553164E-3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="9"/>
+        <v>1.0123849069776582E-3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="10"/>
+        <v>1012</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="11"/>
+        <v>1.0119999999999999E-3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="12"/>
+        <v>2.0239999999999998E-3</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="13"/>
+        <v>494.07114624505937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="7"/>
+        <v>523.25113060119725</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="8"/>
+        <v>1.911128216485715E-3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="9"/>
+        <v>9.555641082428575E-4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="10"/>
+        <v>956</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="11"/>
+        <v>9.5599999999999993E-4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="12"/>
+        <v>1.9119999999999999E-3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="13"/>
+        <v>523.01255230125525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="7"/>
+        <v>554.36526195374415</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="8"/>
+        <v>1.803864831782045E-3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="9"/>
+        <v>9.019324158910225E-4</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="10"/>
+        <v>902</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="11"/>
+        <v>9.0199999999999992E-4</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="12"/>
+        <v>1.8039999999999998E-3</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="13"/>
+        <v>554.32372505543242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="7"/>
+        <v>587.32953583481515</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="8"/>
+        <v>1.7026216782689563E-3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="9"/>
+        <v>8.5131083913447814E-4</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="10"/>
+        <v>851</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="11"/>
+        <v>8.5099999999999998E-4</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="12"/>
+        <v>1.702E-3</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="13"/>
+        <v>587.54406580493537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="7"/>
+        <v>622.25396744416184</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="8"/>
+        <v>1.6070608663330626E-3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="9"/>
+        <v>8.0353043316653129E-4</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="10"/>
+        <v>804</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="11"/>
+        <v>8.0399999999999992E-4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="12"/>
+        <v>1.6079999999999998E-3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="13"/>
+        <v>621.8905472636817</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="7"/>
+        <v>659.25511382573984</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="8"/>
+        <v>1.5168634706477664E-3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="9"/>
+        <v>7.5843173532388322E-4</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="10"/>
+        <v>758</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="11"/>
+        <v>7.5799999999999999E-4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="12"/>
+        <v>1.516E-3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="13"/>
+        <v>659.63060686015831</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="7"/>
+        <v>698.45646286600777</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="8"/>
+        <v>1.4317284657896286E-3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="9"/>
+        <v>7.158642328948143E-4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="10"/>
+        <v>716</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="11"/>
+        <v>7.1599999999999995E-4</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="12"/>
+        <v>1.4319999999999999E-3</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="13"/>
+        <v>698.32402234636879</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="7"/>
+        <v>739.9888454232688</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="8"/>
+        <v>1.3513717215940012E-3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="9"/>
+        <v>6.7568586079700061E-4</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="10"/>
+        <v>676</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="11"/>
+        <v>6.7599999999999995E-4</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="12"/>
+        <v>1.3519999999999999E-3</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="13"/>
+        <v>739.64497041420123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="7"/>
+        <v>783.99087196349853</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="8"/>
+        <v>1.2755250548970149E-3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="9"/>
+        <v>6.3776252744850745E-4</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="10"/>
+        <v>638</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="11"/>
+        <v>6.38E-4</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="12"/>
+        <v>1.276E-3</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="13"/>
+        <v>783.69905956112848</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="7"/>
+        <v>830.60939515989025</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="8"/>
+        <v>1.2039353344991991E-3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="9"/>
+        <v>6.0196766724959956E-4</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="10"/>
+        <v>602</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="11"/>
+        <v>6.02E-4</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="12"/>
+        <v>1.204E-3</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="13"/>
+        <v>830.56478405315613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>